<commit_message>
Updating Selenium framework code
</commit_message>
<xml_diff>
--- a/src/main/java/com/FP/data/Data.xlsx
+++ b/src/main/java/com/FP/data/Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Framework_New\Framework\Framework\src\main\java\com\FP\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Java-Selenium-Framework\src\main\java\com\FP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660FE340-00B2-4884-814B-3C1583F095C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14145" windowHeight="5655" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="13" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC1" sheetId="1" r:id="rId1"/>
@@ -30,6 +31,7 @@
     <sheet name="Save As Template" sheetId="17" r:id="rId16"/>
     <sheet name="Named Entity Train" sheetId="18" r:id="rId17"/>
     <sheet name="RULES FUNCTIONALITY" sheetId="20" r:id="rId18"/>
+    <sheet name="Test Sheet" sheetId="22" r:id="rId19"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="334">
   <si>
     <t>Email</t>
   </si>
@@ -1038,12 +1040,24 @@
   </si>
   <si>
     <t>Count of the number of tagged occurrences for single occurrence for ORGANIZATION</t>
+  </si>
+  <si>
+    <t>Text to search</t>
+  </si>
+  <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>Text to verify</t>
+  </si>
+  <si>
+    <t>Selenium WebDriver</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1061,7 +1075,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1077,6 +1091,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1119,7 +1139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1182,6 +1202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1495,19 +1516,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="18.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1515,7 +1536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1530,27 +1551,27 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.109375" customWidth="1"/>
+    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="34" customWidth="1"/>
     <col min="10" max="10" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>62</v>
       </c>
@@ -1582,7 +1603,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>293</v>
       </c>
@@ -1621,47 +1642,47 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
     <sheetView topLeftCell="Y1" workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.140625" customWidth="1"/>
-    <col min="6" max="6" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.109375" customWidth="1"/>
+    <col min="6" max="6" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5546875" customWidth="1"/>
     <col min="9" max="9" width="27" customWidth="1"/>
-    <col min="10" max="10" width="28.140625" customWidth="1"/>
-    <col min="11" max="11" width="27.7109375" customWidth="1"/>
-    <col min="12" max="13" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="50.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="30.5703125" customWidth="1"/>
-    <col min="16" max="16" width="34.42578125" customWidth="1"/>
+    <col min="10" max="10" width="28.109375" customWidth="1"/>
+    <col min="11" max="11" width="27.6640625" customWidth="1"/>
+    <col min="12" max="13" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="50.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.5546875" customWidth="1"/>
+    <col min="16" max="16" width="34.44140625" customWidth="1"/>
     <col min="17" max="17" width="36" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.85546875" customWidth="1"/>
-    <col min="20" max="20" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="25.42578125" customWidth="1"/>
-    <col min="22" max="22" width="37.140625" customWidth="1"/>
-    <col min="23" max="23" width="24.42578125" customWidth="1"/>
-    <col min="24" max="24" width="25.7109375" customWidth="1"/>
+    <col min="18" max="18" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.88671875" customWidth="1"/>
+    <col min="20" max="20" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="25.44140625" customWidth="1"/>
+    <col min="22" max="22" width="37.109375" customWidth="1"/>
+    <col min="23" max="23" width="24.44140625" customWidth="1"/>
+    <col min="24" max="24" width="25.6640625" customWidth="1"/>
     <col min="25" max="25" width="22" customWidth="1"/>
-    <col min="26" max="26" width="27.140625" customWidth="1"/>
-    <col min="27" max="27" width="66.5703125" customWidth="1"/>
-    <col min="28" max="28" width="22.5703125" customWidth="1"/>
+    <col min="26" max="26" width="27.109375" customWidth="1"/>
+    <col min="27" max="27" width="66.5546875" customWidth="1"/>
+    <col min="28" max="28" width="22.5546875" customWidth="1"/>
     <col min="29" max="29" width="13" customWidth="1"/>
-    <col min="30" max="30" width="17.85546875" customWidth="1"/>
+    <col min="30" max="30" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="13" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>84</v>
       </c>
@@ -1753,7 +1774,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>96</v>
       </c>
@@ -1852,32 +1873,32 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" customWidth="1"/>
+    <col min="6" max="6" width="29.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="32" customWidth="1"/>
-    <col min="8" max="8" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1"/>
-    <col min="11" max="11" width="28.42578125" customWidth="1"/>
-    <col min="12" max="12" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" customWidth="1"/>
+    <col min="11" max="11" width="28.44140625" customWidth="1"/>
+    <col min="12" max="12" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="52" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>125</v>
       </c>
@@ -1924,7 +1945,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>126</v>
       </c>
@@ -1978,26 +1999,26 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" customWidth="1"/>
-    <col min="7" max="7" width="54.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.88671875" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5546875" customWidth="1"/>
+    <col min="6" max="6" width="27.44140625" customWidth="1"/>
+    <col min="7" max="7" width="54.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>61</v>
       </c>
@@ -2020,7 +2041,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>144</v>
       </c>
@@ -2050,24 +2071,24 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" customWidth="1"/>
-    <col min="6" max="6" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" customWidth="1"/>
+    <col min="5" max="5" width="28.44140625" customWidth="1"/>
+    <col min="6" max="6" width="54.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>61</v>
       </c>
@@ -2087,7 +2108,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>175</v>
       </c>
@@ -2114,27 +2135,27 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" customWidth="1"/>
-    <col min="3" max="3" width="40.28515625" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" customWidth="1"/>
-    <col min="6" max="6" width="36.42578125" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" customWidth="1"/>
-    <col min="9" max="9" width="37.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.109375" customWidth="1"/>
+    <col min="2" max="2" width="32.5546875" customWidth="1"/>
+    <col min="3" max="3" width="40.33203125" customWidth="1"/>
+    <col min="4" max="4" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.109375" customWidth="1"/>
+    <col min="6" max="6" width="36.44140625" customWidth="1"/>
+    <col min="7" max="7" width="20.44140625" customWidth="1"/>
+    <col min="8" max="8" width="28.109375" customWidth="1"/>
+    <col min="9" max="9" width="37.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>148</v>
       </c>
@@ -2163,7 +2184,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>149</v>
       </c>
@@ -2199,29 +2220,29 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.140625" customWidth="1"/>
-    <col min="2" max="2" width="66.5703125" customWidth="1"/>
-    <col min="3" max="3" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.42578125" customWidth="1"/>
-    <col min="5" max="5" width="36.28515625" customWidth="1"/>
-    <col min="6" max="6" width="30.85546875" customWidth="1"/>
+    <col min="1" max="1" width="37.109375" customWidth="1"/>
+    <col min="2" max="2" width="66.5546875" customWidth="1"/>
+    <col min="3" max="3" width="43.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.44140625" customWidth="1"/>
+    <col min="5" max="5" width="36.33203125" customWidth="1"/>
+    <col min="6" max="6" width="30.88671875" customWidth="1"/>
     <col min="7" max="7" width="73" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" customWidth="1"/>
-    <col min="9" max="9" width="28.28515625" customWidth="1"/>
+    <col min="8" max="8" width="34.44140625" customWidth="1"/>
+    <col min="9" max="9" width="28.33203125" customWidth="1"/>
     <col min="10" max="11" width="70" customWidth="1"/>
-    <col min="12" max="12" width="46.42578125" customWidth="1"/>
+    <col min="12" max="12" width="46.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>163</v>
       </c>
@@ -2259,7 +2280,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="12" customFormat="1" ht="350.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="12" customFormat="1" ht="350.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>149</v>
       </c>
@@ -2304,37 +2325,37 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="T1" sqref="T1:W2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" customWidth="1"/>
-    <col min="4" max="4" width="37.85546875" customWidth="1"/>
-    <col min="5" max="5" width="34.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.109375" customWidth="1"/>
+    <col min="4" max="4" width="37.88671875" customWidth="1"/>
+    <col min="5" max="5" width="34.33203125" customWidth="1"/>
     <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="28" customWidth="1"/>
-    <col min="9" max="9" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29" customWidth="1"/>
-    <col min="11" max="11" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="19" customWidth="1"/>
-    <col min="15" max="15" width="21.85546875" customWidth="1"/>
-    <col min="16" max="16" width="28.7109375" customWidth="1"/>
-    <col min="18" max="18" width="22.5703125" customWidth="1"/>
-    <col min="20" max="20" width="18.28515625" customWidth="1"/>
-    <col min="21" max="21" width="21.5703125" customWidth="1"/>
-    <col min="22" max="22" width="18.140625" customWidth="1"/>
-    <col min="23" max="23" width="17.140625" customWidth="1"/>
+    <col min="15" max="15" width="21.88671875" customWidth="1"/>
+    <col min="16" max="16" width="28.6640625" customWidth="1"/>
+    <col min="18" max="18" width="22.5546875" customWidth="1"/>
+    <col min="20" max="20" width="18.33203125" customWidth="1"/>
+    <col min="21" max="21" width="21.5546875" customWidth="1"/>
+    <col min="22" max="22" width="18.109375" customWidth="1"/>
+    <col min="23" max="23" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>173</v>
       </c>
@@ -2393,7 +2414,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>172</v>
       </c>
@@ -2459,28 +2480,28 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36.85546875" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" customWidth="1"/>
-    <col min="5" max="5" width="36.5703125" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" customWidth="1"/>
-    <col min="8" max="8" width="49.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.88671875" customWidth="1"/>
+    <col min="3" max="3" width="36.88671875" customWidth="1"/>
+    <col min="4" max="4" width="31.88671875" customWidth="1"/>
+    <col min="5" max="5" width="36.5546875" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" customWidth="1"/>
+    <col min="7" max="7" width="27.88671875" customWidth="1"/>
+    <col min="8" max="8" width="49.109375" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="23" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="23" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>256</v>
       </c>
@@ -2512,7 +2533,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>257</v>
       </c>
@@ -2550,20 +2571,55 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3C481A4-19D0-412A-9343-FA644D7776B5}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
+        <v>330</v>
+      </c>
+      <c r="B1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -2571,7 +2627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2585,20 +2641,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="5" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="5" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -2606,7 +2662,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -2621,48 +2677,48 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="46" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.5703125" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="33.5546875" customWidth="1"/>
+    <col min="6" max="6" width="26.109375" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
-    <col min="8" max="8" width="29.140625" customWidth="1"/>
-    <col min="9" max="9" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.109375" customWidth="1"/>
+    <col min="9" max="9" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27" customWidth="1"/>
-    <col min="12" max="12" width="27.5703125" customWidth="1"/>
-    <col min="13" max="13" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.5546875" customWidth="1"/>
+    <col min="13" max="13" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.42578125" customWidth="1"/>
+    <col min="16" max="16" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.44140625" customWidth="1"/>
     <col min="18" max="18" width="19" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="28.42578125" customWidth="1"/>
-    <col min="23" max="23" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.44140625" customWidth="1"/>
+    <col min="23" max="23" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="19" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="28.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="13" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" s="13" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>12</v>
       </c>
@@ -2757,7 +2813,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>236</v>
       </c>
@@ -2859,21 +2915,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>70</v>
       </c>
@@ -2884,7 +2940,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -2902,23 +2958,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.42578125" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.44140625" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
@@ -2935,7 +2991,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -2959,23 +3015,23 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>24</v>
       </c>
@@ -2993,7 +3049,7 @@
       </c>
       <c r="F1" s="8"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>25</v>
       </c>
@@ -3018,33 +3074,33 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" style="12" customWidth="1"/>
-    <col min="11" max="11" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" style="12" customWidth="1"/>
+    <col min="11" max="11" width="35.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="20" width="27" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="40.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="40.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>31</v>
       </c>
@@ -3121,7 +3177,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="13" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" s="13" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>32</v>
       </c>
@@ -3205,26 +3261,26 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>49</v>
       </c>
@@ -3250,7 +3306,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="13" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>51</v>
       </c>

</xml_diff>